<commit_message>
Extracted Adj. Rand & Error Rate from all candidate models for IMFA/OMFA/MIFA/MFA runs to demonstrate that BICM doesn't always find the optimal clustering. Fixed two minor bugs related to G=1/clust.ind and summary/print functions.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4638" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4638" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Real Data" sheetId="5" r:id="rId1"/>
-    <sheet name="Olive" sheetId="4" r:id="rId2"/>
-    <sheet name="Benchmarking" sheetId="1" r:id="rId3"/>
-    <sheet name="Simulation Study" sheetId="6" r:id="rId4"/>
-    <sheet name="PGMM" sheetId="3" r:id="rId5"/>
+    <sheet name="Supplementary Olive" sheetId="7" r:id="rId2"/>
+    <sheet name="Olive" sheetId="4" r:id="rId3"/>
+    <sheet name="Benchmarking" sheetId="1" r:id="rId4"/>
+    <sheet name="Simulation Study" sheetId="6" r:id="rId5"/>
+    <sheet name="PGMM" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="120">
   <si>
     <t>Data</t>
   </si>
@@ -328,6 +329,66 @@
   </si>
   <si>
     <t>Support for G=4, alpha.d1=3, alpha.d2=6</t>
+  </si>
+  <si>
+    <t>BICM</t>
+  </si>
+  <si>
+    <t>Q=5 gives best clustering</t>
+  </si>
+  <si>
+    <t>Q=4 gives best clustering</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>3, 6, 3</t>
+  </si>
+  <si>
+    <t>2, 6, 2, 3</t>
+  </si>
+  <si>
+    <t>2, 6, 2, 2, 3</t>
+  </si>
+  <si>
+    <t>2, 2, 1, 2, 2, 3</t>
+  </si>
+  <si>
+    <t>2, 2, 2, 2, 1, 2, 6</t>
+  </si>
+  <si>
+    <t>2, 6, 1, 2, 2, 2, 2, 2</t>
+  </si>
+  <si>
+    <t>2, 6, 2, 1, 2, 1, 2, 2, 2</t>
+  </si>
+  <si>
+    <t>Q (Cinzia)</t>
+  </si>
+  <si>
+    <t>3, 3, 6</t>
+  </si>
+  <si>
+    <t>6, 2, 2, 3</t>
+  </si>
+  <si>
+    <t>BICM, Best Area, Best Cinzia</t>
+  </si>
+  <si>
+    <t>Best Area, Best Cinzia</t>
+  </si>
+  <si>
+    <t>Best Area</t>
+  </si>
+  <si>
+    <t>Best Cinzia</t>
+  </si>
+  <si>
+    <t>G=4 or 5 gives best clustering</t>
+  </si>
+  <si>
+    <t>G=9, Q=4 gives best clustering</t>
   </si>
 </sst>
 </file>
@@ -375,7 +436,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -639,9 +700,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,9 +754,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -742,6 +797,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="A8" activeCellId="1" sqref="A5:A6 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1112,13 +1173,13 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="45"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -1242,7 +1303,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1271,7 +1332,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="58" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1331,7 +1392,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1354,27 +1415,51 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="40">
+      <c r="B9" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="39">
         <v>25000</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
-      <c r="G9" s="40">
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39">
+        <v>0</v>
+      </c>
+      <c r="G9" s="39">
         <v>4</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
       <c r="K9" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1390,10 +1475,2337 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A85" sqref="A85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.68359375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.9453125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83984375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.23980000000000001</v>
+      </c>
+      <c r="G2" s="5">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="H2" s="5">
+        <v>62.94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.29049999999999998</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.32429999999999998</v>
+      </c>
+      <c r="G3" s="5">
+        <v>58.220000000000006</v>
+      </c>
+      <c r="H3" s="5">
+        <v>50.519999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.2969</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.33130000000000004</v>
+      </c>
+      <c r="G4" s="5">
+        <v>59.62</v>
+      </c>
+      <c r="H4" s="5">
+        <v>52.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.45629999999999998</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.49959999999999999</v>
+      </c>
+      <c r="G5" s="5">
+        <v>42.480000000000004</v>
+      </c>
+      <c r="H5" s="5">
+        <v>34.619999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.49430000000000002</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.54010000000000002</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42.83</v>
+      </c>
+      <c r="H6" s="5">
+        <v>34.619999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.51639999999999997</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.5665</v>
+      </c>
+      <c r="G7" s="5">
+        <v>37.24</v>
+      </c>
+      <c r="H7" s="5">
+        <v>28.85</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.56540000000000001</v>
+      </c>
+      <c r="G8" s="3">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="H8" s="3">
+        <v>29.020000000000003</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.19270000000000001</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="G9" s="5">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="H9" s="5">
+        <v>66.430000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.27210000000000001</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.30420000000000003</v>
+      </c>
+      <c r="G10" s="5">
+        <v>62.76</v>
+      </c>
+      <c r="H10" s="5">
+        <v>55.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.34660000000000002</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.38550000000000001</v>
+      </c>
+      <c r="G11" s="5">
+        <v>54.19</v>
+      </c>
+      <c r="H11" s="5">
+        <v>46.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.43309999999999998</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.47470000000000001</v>
+      </c>
+      <c r="G12" s="5">
+        <v>43.36</v>
+      </c>
+      <c r="H12" s="5">
+        <v>35.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.62560000000000004</v>
+      </c>
+      <c r="G13" s="5">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="H13" s="5">
+        <v>29.19</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.56540000000000001</v>
+      </c>
+      <c r="G14" s="4">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="H14" s="5">
+        <v>29.02</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.56059999999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.61040000000000005</v>
+      </c>
+      <c r="G15" s="3">
+        <v>39.51</v>
+      </c>
+      <c r="H15" s="3">
+        <v>31.12</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>43.53</v>
+      </c>
+      <c r="H16" s="6">
+        <v>43.53</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.7571</v>
+      </c>
+      <c r="G17" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H17" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.82020000000000004</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="G18" s="5">
+        <v>15.91</v>
+      </c>
+      <c r="H18" s="5">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.9304</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.94259999999999999</v>
+      </c>
+      <c r="G19" s="5">
+        <v>10.49</v>
+      </c>
+      <c r="H19" s="5">
+        <v>6.99</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="G20" s="5">
+        <v>15.38</v>
+      </c>
+      <c r="H20" s="5">
+        <v>6.99</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="5">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.9284</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.94310000000000005</v>
+      </c>
+      <c r="G21" s="5">
+        <v>11.01</v>
+      </c>
+      <c r="H21" s="5">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.68010000000000004</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.6865</v>
+      </c>
+      <c r="G22" s="5">
+        <v>23.95</v>
+      </c>
+      <c r="H22" s="5">
+        <v>19.760000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.5474</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.59670000000000001</v>
+      </c>
+      <c r="G23" s="5">
+        <v>42.31</v>
+      </c>
+      <c r="H23" s="5">
+        <v>33.92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="3">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.86240000000000006</v>
+      </c>
+      <c r="G24" s="3">
+        <v>21.84</v>
+      </c>
+      <c r="H24" s="3">
+        <v>13.46</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H25" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H26" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H27" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H28" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>4</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H29" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H30" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>43.53</v>
+      </c>
+      <c r="H31" s="5">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G32" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H32" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G33" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H33" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G34" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H34" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F35" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G35" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H35" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2</v>
+      </c>
+      <c r="C36" s="5">
+        <v>4</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G36" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H36" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5">
+        <v>5</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G37" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H37" s="5">
+        <v>26.05</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="5">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="G38" s="5">
+        <v>17.13</v>
+      </c>
+      <c r="H38" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.51259999999999994</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="G39" s="5">
+        <v>18.88</v>
+      </c>
+      <c r="H39" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="5">
+        <v>3</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0.47420000000000001</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.39639999999999997</v>
+      </c>
+      <c r="G40" s="5">
+        <v>26.4</v>
+      </c>
+      <c r="H40" s="5">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="5">
+        <v>3</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.63719999999999999</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.63959999999999995</v>
+      </c>
+      <c r="G41" s="5">
+        <v>23.78</v>
+      </c>
+      <c r="H41" s="5">
+        <v>23.78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="5">
+        <v>3</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0.70420000000000005</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="G42" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="H42" s="5">
+        <v>26.57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5">
+        <v>3</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0.61439999999999995</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.61619999999999997</v>
+      </c>
+      <c r="G43" s="5">
+        <v>24.83</v>
+      </c>
+      <c r="H43" s="5">
+        <v>24.83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="5">
+        <v>3</v>
+      </c>
+      <c r="C44" s="5">
+        <v>5</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0.64929999999999999</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.65329999999999999</v>
+      </c>
+      <c r="G44" s="5">
+        <v>23.07</v>
+      </c>
+      <c r="H44" s="5">
+        <v>23.08</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="5">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5">
+        <v>6</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0.49130000000000001</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.41460000000000002</v>
+      </c>
+      <c r="G45" s="5">
+        <v>21.85</v>
+      </c>
+      <c r="H45" s="5">
+        <v>26.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="5">
+        <v>4</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0.69259999999999999</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.61329999999999996</v>
+      </c>
+      <c r="G46" s="5">
+        <v>18.88</v>
+      </c>
+      <c r="H46" s="5">
+        <v>18.88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="5">
+        <v>4</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0.65410000000000001</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0.57210000000000005</v>
+      </c>
+      <c r="G47" s="5">
+        <v>26.4</v>
+      </c>
+      <c r="H47" s="5">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="5">
+        <v>4</v>
+      </c>
+      <c r="C48" s="5">
+        <v>2</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0.58940000000000003</v>
+      </c>
+      <c r="G48" s="5">
+        <v>22.03</v>
+      </c>
+      <c r="H48" s="5">
+        <v>22.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="5">
+        <v>4</v>
+      </c>
+      <c r="C49" s="5">
+        <v>3</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.58609999999999995</v>
+      </c>
+      <c r="G49" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="H49" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="5">
+        <v>4</v>
+      </c>
+      <c r="C50" s="5">
+        <v>4</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0.67510000000000003</v>
+      </c>
+      <c r="F50" s="5">
+        <v>0.59489999999999998</v>
+      </c>
+      <c r="G50" s="5">
+        <v>20.8</v>
+      </c>
+      <c r="H50" s="5">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="5">
+        <v>4</v>
+      </c>
+      <c r="C51" s="5">
+        <v>5</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0.47849999999999998</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0.52470000000000006</v>
+      </c>
+      <c r="G51" s="5">
+        <v>30.07</v>
+      </c>
+      <c r="H51" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="5">
+        <v>4</v>
+      </c>
+      <c r="C52" s="5">
+        <v>6</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0.59019999999999995</v>
+      </c>
+      <c r="G52" s="5">
+        <v>30.42</v>
+      </c>
+      <c r="H52" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="5">
+        <v>5</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0.62229999999999996</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0.66979999999999995</v>
+      </c>
+      <c r="G53" s="5">
+        <v>27.45</v>
+      </c>
+      <c r="H53" s="5">
+        <v>19.579999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="5">
+        <v>5</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="5">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F54" s="5">
+        <v>0.62760000000000005</v>
+      </c>
+      <c r="G54" s="5">
+        <v>34.97</v>
+      </c>
+      <c r="H54" s="5">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="5">
+        <v>5</v>
+      </c>
+      <c r="C55" s="5">
+        <v>2</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0.59750000000000003</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="G55" s="5">
+        <v>30.59</v>
+      </c>
+      <c r="H55" s="5">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="5">
+        <v>5</v>
+      </c>
+      <c r="C56" s="5">
+        <v>3</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0.59750000000000003</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="G56" s="5">
+        <v>30.59</v>
+      </c>
+      <c r="H56" s="5">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="5">
+        <v>5</v>
+      </c>
+      <c r="C57" s="5">
+        <v>4</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0.60070000000000001</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0.64839999999999998</v>
+      </c>
+      <c r="G57" s="5">
+        <v>30.07</v>
+      </c>
+      <c r="H57" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="5">
+        <v>5</v>
+      </c>
+      <c r="C58" s="5">
+        <v>5</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0.60119999999999996</v>
+      </c>
+      <c r="F58" s="5">
+        <v>0.64890000000000003</v>
+      </c>
+      <c r="G58" s="5">
+        <v>30.24</v>
+      </c>
+      <c r="H58" s="5">
+        <v>22.38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="5">
+        <v>5</v>
+      </c>
+      <c r="C59" s="5">
+        <v>6</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0.59370000000000001</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0.58960000000000001</v>
+      </c>
+      <c r="G59" s="5">
+        <v>32.17</v>
+      </c>
+      <c r="H59" s="5">
+        <v>29.37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="5">
+        <v>6</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0.50529999999999997</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0.54620000000000002</v>
+      </c>
+      <c r="G60" s="5">
+        <v>36.01</v>
+      </c>
+      <c r="H60" s="5">
+        <v>28.15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="5">
+        <v>6</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0.49159999999999998</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0.48459999999999998</v>
+      </c>
+      <c r="G61" s="5">
+        <v>39.159999999999997</v>
+      </c>
+      <c r="H61" s="5">
+        <v>35.31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="5">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5">
+        <v>2</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0.4748</v>
+      </c>
+      <c r="F62" s="5">
+        <v>0.46789999999999998</v>
+      </c>
+      <c r="G62" s="5">
+        <v>42.48</v>
+      </c>
+      <c r="H62" s="5">
+        <v>38.29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="5">
+        <v>6</v>
+      </c>
+      <c r="C63" s="5">
+        <v>3</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0.52690000000000003</v>
+      </c>
+      <c r="F63" s="5">
+        <v>0.57050000000000001</v>
+      </c>
+      <c r="G63" s="5">
+        <v>34.97</v>
+      </c>
+      <c r="H63" s="5">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="5">
+        <v>6</v>
+      </c>
+      <c r="C64" s="5">
+        <v>4</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="5">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F64" s="5">
+        <v>0.6613</v>
+      </c>
+      <c r="G64" s="5">
+        <v>28.5</v>
+      </c>
+      <c r="H64" s="5">
+        <v>20.63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="5">
+        <v>6</v>
+      </c>
+      <c r="C65" s="5">
+        <v>5</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0.51429999999999998</v>
+      </c>
+      <c r="F65" s="5">
+        <v>0.56430000000000002</v>
+      </c>
+      <c r="G65" s="5">
+        <v>37.590000000000003</v>
+      </c>
+      <c r="H65" s="5">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" s="5">
+        <v>6</v>
+      </c>
+      <c r="C66" s="5">
+        <v>6</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0.59230000000000005</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0.58809999999999996</v>
+      </c>
+      <c r="G66" s="5">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="H66" s="5">
+        <v>29.55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="5">
+        <v>7</v>
+      </c>
+      <c r="C67" s="5">
+        <v>0</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="5">
+        <v>0.4713</v>
+      </c>
+      <c r="F67" s="5">
+        <v>0.50990000000000002</v>
+      </c>
+      <c r="G67" s="5">
+        <v>41.96</v>
+      </c>
+      <c r="H67" s="5">
+        <v>34.090000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="5">
+        <v>7</v>
+      </c>
+      <c r="C68" s="5">
+        <v>1</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0.46160000000000001</v>
+      </c>
+      <c r="F68" s="5">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="G68" s="5">
+        <v>44.23</v>
+      </c>
+      <c r="H68" s="5">
+        <v>35.840000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" s="5">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5">
+        <v>2</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="5">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="F69" s="5">
+        <v>0.3911</v>
+      </c>
+      <c r="G69" s="5">
+        <v>45.8</v>
+      </c>
+      <c r="H69" s="5">
+        <v>37.409999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="5">
+        <v>7</v>
+      </c>
+      <c r="C70" s="5">
+        <v>3</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="5">
+        <v>0.5262</v>
+      </c>
+      <c r="F70" s="5">
+        <v>0.56969999999999998</v>
+      </c>
+      <c r="G70" s="5">
+        <v>35.14</v>
+      </c>
+      <c r="H70" s="5">
+        <v>27.27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="5">
+        <v>7</v>
+      </c>
+      <c r="C71" s="5">
+        <v>4</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.60909999999999997</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0.65720000000000001</v>
+      </c>
+      <c r="G71" s="5">
+        <v>29.02</v>
+      </c>
+      <c r="H71" s="5">
+        <v>21.15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="5">
+        <v>7</v>
+      </c>
+      <c r="C72" s="5">
+        <v>5</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.51319999999999999</v>
+      </c>
+      <c r="F72" s="5">
+        <v>0.56320000000000003</v>
+      </c>
+      <c r="G72" s="5">
+        <v>37.76</v>
+      </c>
+      <c r="H72" s="5">
+        <v>29.37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="5">
+        <v>7</v>
+      </c>
+      <c r="C73" s="5">
+        <v>6</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.47489999999999999</v>
+      </c>
+      <c r="F73" s="5">
+        <v>0.52090000000000003</v>
+      </c>
+      <c r="G73" s="5">
+        <v>30.94</v>
+      </c>
+      <c r="H73" s="5">
+        <v>23.08</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" s="5">
+        <v>8</v>
+      </c>
+      <c r="C74" s="5">
+        <v>0</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0.47549999999999998</v>
+      </c>
+      <c r="G74" s="5">
+        <v>50</v>
+      </c>
+      <c r="H74" s="5">
+        <v>41.61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="5">
+        <v>8</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0.42759999999999998</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="G75" s="5">
+        <v>53.32</v>
+      </c>
+      <c r="H75" s="5">
+        <v>44.93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="5">
+        <v>8</v>
+      </c>
+      <c r="C76" s="5">
+        <v>2</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="5">
+        <v>0.38919999999999999</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0.42830000000000001</v>
+      </c>
+      <c r="G76" s="5">
+        <v>47.2</v>
+      </c>
+      <c r="H76" s="5">
+        <v>38.81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" s="5">
+        <v>8</v>
+      </c>
+      <c r="C77" s="5">
+        <v>3</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0.50380000000000003</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0.55020000000000002</v>
+      </c>
+      <c r="G77" s="5">
+        <v>42.48</v>
+      </c>
+      <c r="H77" s="5">
+        <v>34.619999999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" s="5">
+        <v>8</v>
+      </c>
+      <c r="C78" s="5">
+        <v>4</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="5">
+        <v>0.47770000000000001</v>
+      </c>
+      <c r="F78" s="5">
+        <v>0.52239999999999998</v>
+      </c>
+      <c r="G78" s="5">
+        <v>43.18</v>
+      </c>
+      <c r="H78" s="5">
+        <v>34.97</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" s="5">
+        <v>8</v>
+      </c>
+      <c r="C79" s="5">
+        <v>5</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="F79" s="5">
+        <v>0.58279999999999998</v>
+      </c>
+      <c r="G79" s="5">
+        <v>33.39</v>
+      </c>
+      <c r="H79" s="5">
+        <v>30.24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="5">
+        <v>8</v>
+      </c>
+      <c r="C80" s="5">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" s="5">
+        <v>0.57809999999999995</v>
+      </c>
+      <c r="F80" s="5">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="G80" s="5">
+        <v>35.659999999999997</v>
+      </c>
+      <c r="H80" s="5">
+        <v>32.869999999999997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="5">
+        <v>9</v>
+      </c>
+      <c r="C81" s="5">
+        <v>0</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0.38629999999999998</v>
+      </c>
+      <c r="F81" s="5">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="G81" s="5">
+        <v>51.05</v>
+      </c>
+      <c r="H81" s="5">
+        <v>42.66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" s="5">
+        <v>9</v>
+      </c>
+      <c r="C82" s="5">
+        <v>1</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="5">
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="F82" s="5">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="G82" s="5">
+        <v>51.75</v>
+      </c>
+      <c r="H82" s="5">
+        <v>43.36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="5">
+        <v>9</v>
+      </c>
+      <c r="C83" s="5">
+        <v>2</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0.34589999999999999</v>
+      </c>
+      <c r="F83" s="5">
+        <v>0.38469999999999999</v>
+      </c>
+      <c r="G83" s="5">
+        <v>51.57</v>
+      </c>
+      <c r="H83" s="5">
+        <v>43.18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="5">
+        <v>9</v>
+      </c>
+      <c r="C84" s="5">
+        <v>3</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0.48089999999999999</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0.52590000000000003</v>
+      </c>
+      <c r="G84" s="5">
+        <v>44.41</v>
+      </c>
+      <c r="H84" s="5">
+        <v>36.54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="5">
+        <v>9</v>
+      </c>
+      <c r="C85" s="5">
+        <v>4</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="5">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0.96240000000000003</v>
+      </c>
+      <c r="G85" s="5">
+        <v>17.48</v>
+      </c>
+      <c r="H85" s="5">
+        <v>9.27</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="5">
+        <v>9</v>
+      </c>
+      <c r="C86" s="5">
+        <v>5</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="5">
+        <v>0.48409999999999997</v>
+      </c>
+      <c r="F86" s="5">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="G86" s="5">
+        <v>33.57</v>
+      </c>
+      <c r="H86" s="5">
+        <v>28.85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A87" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="3">
+        <v>9</v>
+      </c>
+      <c r="C87" s="3">
+        <v>6</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="3">
+        <v>0.59079999999999999</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="G87" s="3">
+        <v>32.69</v>
+      </c>
+      <c r="H87" s="3">
+        <v>29.55</v>
+      </c>
+      <c r="I87" s="3"/>
+    </row>
+    <row r="88" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C18:D18" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1464,13 +3876,13 @@
       <c r="O1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="45"/>
+      <c r="R1" s="43"/>
     </row>
     <row r="2" spans="1:18" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -1488,7 +3900,7 @@
       <c r="E2" s="14">
         <v>1</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="40">
         <f t="shared" ref="F2:F14" si="0">D2/$D$3</f>
         <v>1.097449010520283</v>
       </c>
@@ -1545,7 +3957,7 @@
       <c r="E3" s="14">
         <v>1</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1602,7 +4014,7 @@
       <c r="E4" s="4">
         <v>7</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="40">
         <f t="shared" si="0"/>
         <v>7.2481442088846517</v>
       </c>
@@ -1633,7 +4045,9 @@
       <c r="O4" s="4">
         <v>28.85</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="Q4" s="19" t="s">
         <v>34</v>
       </c>
@@ -1657,7 +4071,7 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="40">
         <f t="shared" si="0"/>
         <v>1.0252563940063597</v>
       </c>
@@ -1714,7 +4128,7 @@
       <c r="E6" s="4">
         <v>7</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6" s="40">
         <f t="shared" si="0"/>
         <v>5.2613262500068885</v>
       </c>
@@ -1745,7 +4159,9 @@
       <c r="O6" s="5">
         <v>29.02</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="Q6" s="19" t="s">
         <v>36</v>
       </c>
@@ -1754,7 +4170,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1769,7 +4185,7 @@
       <c r="E7" s="4">
         <v>9</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="40">
         <f t="shared" si="0"/>
         <v>3.7739268925762848</v>
       </c>
@@ -1800,7 +4216,9 @@
       <c r="O7" s="6">
         <v>43.53</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="Q7" s="21" t="s">
         <v>37</v>
       </c>
@@ -1809,7 +4227,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1824,7 +4242,7 @@
       <c r="E8" s="4">
         <v>63</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="40">
         <f>D8/$D$3</f>
         <v>18.536539934640885</v>
       </c>
@@ -1855,7 +4273,9 @@
       <c r="O8" s="5">
         <v>26.05</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="18" t="s">
@@ -1873,7 +4293,7 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="40">
         <f t="shared" si="0"/>
         <v>0.13271317487696946</v>
       </c>
@@ -1922,7 +4342,7 @@
       <c r="E10" s="4">
         <v>7</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="40">
         <f t="shared" si="0"/>
         <v>0.60231236808314836</v>
       </c>
@@ -1970,7 +4390,7 @@
       <c r="E11" s="5">
         <v>63</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="40">
         <f t="shared" si="0"/>
         <v>0.16843198739109111</v>
       </c>
@@ -2003,7 +4423,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2015,7 +4435,7 @@
       <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2030,7 +4450,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2042,7 +4462,7 @@
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2057,7 +4477,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2069,7 +4489,7 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2097,7 +4517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
@@ -2105,7 +4525,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2160,13 +4580,13 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="45"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -2512,12 +4932,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2539,47 +4959,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="45"/>
+      <c r="Q1" s="43"/>
     </row>
     <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="53" t="s">
+      <c r="M2" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="51" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="19" t="s">
@@ -2590,19 +5010,19 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
       <c r="P3" s="19" t="s">
         <v>82</v>
       </c>
@@ -2611,41 +5031,41 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="26">
+      <c r="C4" s="45"/>
+      <c r="D4" s="25">
         <v>0.5</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>3</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <v>4</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="28">
         <v>4</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="28">
         <v>4</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="29">
         <v>327.02999999999997</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="30">
         <v>0</v>
       </c>
       <c r="P4" s="19" t="s">
@@ -2656,39 +5076,39 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="26">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="25">
         <v>1</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>3</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="29">
         <v>4</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>4</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="29">
         <v>4</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="29">
         <v>328.11</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="32">
         <v>0</v>
       </c>
       <c r="P5" s="19" t="s">
@@ -2699,39 +5119,39 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="26">
-        <v>5</v>
-      </c>
-      <c r="E6" s="32">
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="25">
+        <v>5</v>
+      </c>
+      <c r="E6" s="31">
         <v>3</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>4</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>4</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="29">
         <v>4</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="29">
         <v>330.5</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="32">
         <v>0</v>
       </c>
       <c r="P6" s="19" t="s">
@@ -2742,39 +5162,39 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="34">
         <v>3</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>4</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="35">
         <v>3</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="35">
         <v>4</v>
       </c>
-      <c r="L7" s="34" t="s">
+      <c r="L7" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="35">
         <v>327.56</v>
       </c>
-      <c r="N7" s="37">
+      <c r="N7" s="36">
         <v>0</v>
       </c>
       <c r="P7" s="21" t="s">
@@ -2785,302 +5205,302 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="26">
+      <c r="C8" s="45"/>
+      <c r="D8" s="25">
         <v>0.5</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="37">
         <v>3</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="38">
-        <v>5</v>
-      </c>
-      <c r="H8" s="26" t="s">
+      <c r="G8" s="37">
+        <v>5</v>
+      </c>
+      <c r="H8" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="38">
-        <v>5</v>
-      </c>
-      <c r="J8" s="26" t="s">
+      <c r="I8" s="37">
+        <v>5</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="38">
-        <v>5</v>
-      </c>
-      <c r="L8" s="26" t="s">
+      <c r="K8" s="37">
+        <v>5</v>
+      </c>
+      <c r="L8" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="26">
         <v>361.66</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="26">
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="25">
         <v>1</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="37">
         <v>3</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="38">
-        <v>5</v>
-      </c>
-      <c r="H9" s="26" t="s">
+      <c r="G9" s="37">
+        <v>5</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="38">
-        <v>5</v>
-      </c>
-      <c r="J9" s="26" t="s">
+      <c r="I9" s="37">
+        <v>5</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="38">
-        <v>5</v>
-      </c>
-      <c r="L9" s="26" t="s">
+      <c r="K9" s="37">
+        <v>5</v>
+      </c>
+      <c r="L9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="31">
         <v>363.06</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="26">
-        <v>5</v>
-      </c>
-      <c r="E10" s="38">
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="25">
+        <v>5</v>
+      </c>
+      <c r="E10" s="37">
         <v>3</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="38">
-        <v>5</v>
-      </c>
-      <c r="H10" s="26" t="s">
+      <c r="G10" s="37">
+        <v>5</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="38">
-        <v>5</v>
-      </c>
-      <c r="J10" s="26" t="s">
+      <c r="I10" s="37">
+        <v>5</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="38">
-        <v>5</v>
-      </c>
-      <c r="L10" s="26" t="s">
+      <c r="K10" s="37">
+        <v>5</v>
+      </c>
+      <c r="L10" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="31">
         <v>367.44</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="34" t="s">
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <v>3</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="38">
-        <v>5</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="37">
+        <v>5</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="38">
-        <v>5</v>
-      </c>
-      <c r="J11" s="26" t="s">
+      <c r="I11" s="37">
+        <v>5</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="38">
-        <v>5</v>
-      </c>
-      <c r="L11" s="26" t="s">
+      <c r="K11" s="37">
+        <v>5</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="34">
         <v>366.57</v>
       </c>
-      <c r="N11" s="37">
+      <c r="N11" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="28">
+      <c r="C12" s="45"/>
+      <c r="D12" s="27">
         <v>0.5</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <v>3</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="29">
-        <v>5</v>
-      </c>
-      <c r="H12" s="28" t="s">
+      <c r="G12" s="28">
+        <v>5</v>
+      </c>
+      <c r="H12" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="29">
-        <v>5</v>
-      </c>
-      <c r="J12" s="28" t="s">
+      <c r="I12" s="28">
+        <v>5</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="29">
-        <v>5</v>
-      </c>
-      <c r="L12" s="28" t="s">
+      <c r="K12" s="28">
+        <v>5</v>
+      </c>
+      <c r="L12" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="29">
         <v>555.82000000000005</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="26">
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="25">
         <v>1</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <v>3</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="30">
-        <v>5</v>
-      </c>
-      <c r="H13" s="26" t="s">
+      <c r="G13" s="29">
+        <v>5</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="30">
-        <v>5</v>
-      </c>
-      <c r="J13" s="26" t="s">
+      <c r="I13" s="29">
+        <v>5</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="30">
-        <v>5</v>
-      </c>
-      <c r="L13" s="26" t="s">
+      <c r="K13" s="29">
+        <v>5</v>
+      </c>
+      <c r="L13" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="30">
+      <c r="M13" s="29">
         <v>558.52</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="26">
-        <v>5</v>
-      </c>
-      <c r="E14" s="32">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="25">
+        <v>5</v>
+      </c>
+      <c r="E14" s="31">
         <v>3</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="30">
-        <v>5</v>
-      </c>
-      <c r="H14" s="26" t="s">
+      <c r="G14" s="29">
+        <v>5</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="30">
-        <v>5</v>
-      </c>
-      <c r="J14" s="26" t="s">
+      <c r="I14" s="29">
+        <v>5</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K14" s="30">
-        <v>5</v>
-      </c>
-      <c r="L14" s="26" t="s">
+      <c r="K14" s="29">
+        <v>5</v>
+      </c>
+      <c r="L14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="M14" s="30">
+      <c r="M14" s="29">
         <v>560.75</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="34" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="34">
         <v>3</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="36">
-        <v>5</v>
-      </c>
-      <c r="H15" s="34" t="s">
+      <c r="G15" s="35">
+        <v>5</v>
+      </c>
+      <c r="H15" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="36">
-        <v>5</v>
-      </c>
-      <c r="J15" s="34" t="s">
+      <c r="I15" s="35">
+        <v>5</v>
+      </c>
+      <c r="J15" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="36">
-        <v>5</v>
-      </c>
-      <c r="L15" s="34" t="s">
+      <c r="K15" s="35">
+        <v>5</v>
+      </c>
+      <c r="L15" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="36">
+      <c r="M15" s="35">
         <v>560.46</v>
       </c>
-      <c r="N15" s="37">
+      <c r="N15" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3107,7 +5527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -3115,7 +5535,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3164,7 +5584,7 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Extensions' section to Notes.pdf incoporating extensions mentioned in WGSL/Insight slides and those included on my to-do-list. Included references. Tried pre-processing Golub data.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -172,9 +172,6 @@
     <t>Empty group in modal clustering</t>
   </si>
   <si>
-    <t>Pre-process</t>
-  </si>
-  <si>
     <t>3, 4, 3, 3</t>
   </si>
   <si>
@@ -389,6 +386,9 @@
   </si>
   <si>
     <t>G=4/5/6 gives best clustering</t>
+  </si>
+  <si>
+    <t>alpha.d1=4, alpha.d2=8</t>
   </si>
 </sst>
 </file>
@@ -763,6 +763,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,24 +824,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1197,44 +1197,44 @@
       <c r="K1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="44"/>
+      <c r="L1" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="58">
+      <c r="A2" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="43">
         <v>50000</v>
       </c>
-      <c r="D2" s="58">
+      <c r="D2" s="43">
         <v>9824.93</v>
       </c>
-      <c r="E2" s="60">
+      <c r="E2" s="45">
         <v>8.9600000000000009</v>
       </c>
-      <c r="F2" s="58">
-        <v>0</v>
-      </c>
-      <c r="G2" s="63">
+      <c r="F2" s="43">
+        <v>0</v>
+      </c>
+      <c r="G2" s="48">
         <v>2</v>
       </c>
-      <c r="H2" s="58">
+      <c r="H2" s="43">
         <v>4</v>
       </c>
-      <c r="I2" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" s="58">
+      <c r="I2" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="43">
         <v>27.78</v>
       </c>
-      <c r="K2" s="62" t="s">
-        <v>80</v>
+      <c r="K2" s="47" t="s">
+        <v>79</v>
       </c>
       <c r="L2" s="19" t="s">
         <v>25</v>
@@ -1269,16 +1269,16 @@
         <v>3</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J3" s="14">
         <v>5.56</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M3" s="20">
         <v>0.75</v>
@@ -1315,7 +1315,9 @@
       <c r="J4" s="8">
         <v>76.19</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="L4" s="19" t="s">
         <v>34</v>
       </c>
@@ -1402,9 +1404,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="K7" s="2"/>
       <c r="L7" s="21" t="s">
         <v>37</v>
       </c>
@@ -1474,9 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1514,10 +1512,10 @@
         <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>30</v>
@@ -1535,74 +1533,74 @@
         <v>3</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="N1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="P1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="44"/>
+      <c r="Q1" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:18" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="58">
+      <c r="A2" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="43">
         <v>50000</v>
       </c>
-      <c r="D2" s="58">
+      <c r="D2" s="43">
         <v>1991.42</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="43">
         <v>1</v>
       </c>
-      <c r="F2" s="59">
+      <c r="F2" s="44">
         <f t="shared" ref="F2:F14" si="0">D2/$D$3</f>
         <v>1.097449010520283</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="45">
         <v>4.5599999999999996</v>
       </c>
-      <c r="H2" s="58">
-        <v>0</v>
-      </c>
-      <c r="I2" s="61" t="s">
+      <c r="H2" s="43">
+        <v>0</v>
+      </c>
+      <c r="I2" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="58">
-        <v>5</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="58">
+      <c r="J2" s="43">
+        <v>5</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="43">
         <v>0.93579999999999997</v>
       </c>
-      <c r="M2" s="58">
+      <c r="M2" s="43">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N2" s="58">
+      <c r="N2" s="43">
         <v>8.57</v>
       </c>
-      <c r="O2" s="58">
+      <c r="O2" s="43">
         <v>0.7</v>
       </c>
-      <c r="P2" s="62" t="s">
-        <v>99</v>
+      <c r="P2" s="47" t="s">
+        <v>98</v>
       </c>
       <c r="Q2" s="19" t="s">
         <v>25</v>
@@ -1659,10 +1657,10 @@
         <v>0.7</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R3" s="20">
         <v>0.75</v>
@@ -1701,7 +1699,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L4" s="4">
         <v>0.51639999999999997</v>
@@ -1716,7 +1714,7 @@
         <v>28.85</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="19" t="s">
         <v>34</v>
@@ -1758,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L5" s="4">
         <v>0.90369999999999995</v>
@@ -1815,7 +1813,7 @@
         <v>6</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L6" s="6">
         <v>0.51529999999999998</v>
@@ -1830,7 +1828,7 @@
         <v>29.02</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>36</v>
@@ -1887,7 +1885,7 @@
         <v>43.53</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q7" s="21" t="s">
         <v>37</v>
@@ -1929,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L8" s="6">
         <v>0.81920000000000004</v>
@@ -1944,7 +1942,7 @@
         <v>26.05</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2077,7 +2075,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L11" s="6">
         <v>0.58860000000000001</v>
@@ -2116,7 +2114,7 @@
         <v>13</v>
       </c>
       <c r="P12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2143,7 +2141,7 @@
         <v>13</v>
       </c>
       <c r="P13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2170,12 +2168,12 @@
         <v>13</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2195,7 +2193,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2223,19 +2221,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>21</v>
@@ -2397,7 +2395,7 @@
         <v>28.85</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2557,7 +2555,7 @@
         <v>29.19</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2586,7 +2584,7 @@
         <v>29.02</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2642,7 +2640,7 @@
         <v>43.53</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2653,10 +2651,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="5">
         <v>0.81920000000000004</v>
@@ -2679,10 +2677,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="5">
         <v>0.82020000000000004</v>
@@ -2705,10 +2703,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="5">
         <v>0.9304</v>
@@ -2723,7 +2721,7 @@
         <v>6.99</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2734,10 +2732,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E20" s="5">
         <v>0.90449999999999997</v>
@@ -2752,7 +2750,7 @@
         <v>6.99</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2763,10 +2761,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="5">
         <v>0.9284</v>
@@ -2789,10 +2787,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="5">
         <v>0.68010000000000004</v>
@@ -2815,10 +2813,10 @@
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="5">
         <v>0.5474</v>
@@ -2841,10 +2839,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="3">
         <v>0.80300000000000005</v>
@@ -3198,7 +3196,7 @@
         <v>26.05</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4449,7 +4447,7 @@
         <v>9.27</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4522,7 +4520,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:K5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4580,10 +4578,10 @@
       <c r="K1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="44"/>
+      <c r="L1" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -4611,7 +4609,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="6">
         <v>79.150000000000006</v>
@@ -4657,7 +4655,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M3" s="20">
         <v>0.75</v>
@@ -4689,13 +4687,13 @@
         <v>5</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="6">
         <v>3.33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>34</v>
@@ -4705,38 +4703,38 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="58">
+      <c r="A5" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="43">
         <v>50000</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="43">
         <v>1991.42</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="45">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F5" s="58">
-        <v>0</v>
-      </c>
-      <c r="G5" s="61" t="s">
+      <c r="F5" s="43">
+        <v>0</v>
+      </c>
+      <c r="G5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="58">
-        <v>5</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="58">
+      <c r="H5" s="43">
+        <v>5</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="43">
         <v>0.7</v>
       </c>
-      <c r="K5" s="62" t="s">
-        <v>90</v>
+      <c r="K5" s="47" t="s">
+        <v>89</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>35</v>
@@ -4777,7 +4775,7 @@
         <v>0.7</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -4956,47 +4954,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="50"/>
+    </row>
+    <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="44"/>
-    </row>
-    <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="54" t="s">
+      <c r="C2" s="61"/>
+      <c r="D2" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="51" t="s">
+      <c r="F2" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G2" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="H2" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="I2" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="K2" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="L2" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="M2" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="58" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="19" t="s">
@@ -5007,31 +5005,31 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
       <c r="P3" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="20">
         <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="46"/>
+      <c r="B4" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="52"/>
       <c r="D4" s="24">
         <v>0.5</v>
       </c>
@@ -5039,25 +5037,25 @@
         <v>3</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="27">
         <v>4</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="27">
         <v>4</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="27">
         <v>4</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M4" s="28">
         <v>327.02999999999997</v>
@@ -5073,8 +5071,8 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="24">
         <v>1</v>
       </c>
@@ -5082,25 +5080,25 @@
         <v>3</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="28">
         <v>4</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="28">
         <v>4</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" s="28">
         <v>4</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M5" s="28">
         <v>328.11</v>
@@ -5116,8 +5114,8 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="24">
         <v>5</v>
       </c>
@@ -5125,25 +5123,25 @@
         <v>3</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="28">
         <v>4</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" s="28">
         <v>4</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" s="28">
         <v>4</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M6" s="28">
         <v>330.5</v>
@@ -5159,34 +5157,34 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="33">
         <v>3</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="34">
         <v>4</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="34">
         <v>3</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="34">
         <v>4</v>
       </c>
       <c r="L7" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M7" s="34">
         <v>327.56</v>
@@ -5202,10 +5200,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="46"/>
+      <c r="B8" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="52"/>
       <c r="D8" s="24">
         <v>0.5</v>
       </c>
@@ -5213,25 +5211,25 @@
         <v>3</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="36">
         <v>5</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="36">
+        <v>5</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="36">
+        <v>5</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="I8" s="36">
-        <v>5</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" s="36">
-        <v>5</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="M8" s="25">
         <v>361.66</v>
@@ -5241,8 +5239,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="24">
         <v>1</v>
       </c>
@@ -5250,25 +5248,25 @@
         <v>3</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="36">
         <v>5</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="36">
         <v>5</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="36">
         <v>5</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M9" s="30">
         <v>363.06</v>
@@ -5278,8 +5276,8 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="24">
         <v>5</v>
       </c>
@@ -5287,25 +5285,25 @@
         <v>3</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="36">
         <v>5</v>
       </c>
       <c r="H10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="36">
+        <v>5</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="36">
+        <v>5</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="I10" s="36">
-        <v>5</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="36">
-        <v>5</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="M10" s="30">
         <v>367.44</v>
@@ -5315,34 +5313,34 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="49"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="36">
         <v>3</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="36">
         <v>5</v>
       </c>
       <c r="H11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="36">
+        <v>5</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="36">
+        <v>5</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="I11" s="36">
-        <v>5</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K11" s="36">
-        <v>5</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="M11" s="33">
         <v>366.57</v>
@@ -5352,10 +5350,10 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="46"/>
+      <c r="B12" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="52"/>
       <c r="D12" s="26">
         <v>0.5</v>
       </c>
@@ -5363,25 +5361,25 @@
         <v>3</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="27">
         <v>5</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="27">
         <v>5</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12" s="27">
         <v>5</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M12" s="28">
         <v>555.82000000000005</v>
@@ -5391,8 +5389,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="24">
         <v>1</v>
       </c>
@@ -5400,25 +5398,25 @@
         <v>3</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="28">
         <v>5</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="28">
         <v>5</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="28">
         <v>5</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M13" s="28">
         <v>558.52</v>
@@ -5428,8 +5426,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="24">
         <v>5</v>
       </c>
@@ -5437,25 +5435,25 @@
         <v>3</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="28">
         <v>5</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="28">
         <v>5</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="28">
         <v>5</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14" s="28">
         <v>560.75</v>
@@ -5465,34 +5463,34 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="33">
         <v>3</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="34">
         <v>5</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="34">
         <v>5</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K15" s="34">
         <v>5</v>
       </c>
       <c r="L15" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M15" s="34">
         <v>560.46</v>
@@ -5681,7 +5679,7 @@
         <v>33.56</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Finished running olive with (10/50/100) additional rows/columns of gaussian noise to check for robustness. Added results to spreadsheet, slides & Notes.pdf
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="128">
   <si>
     <t>Data</t>
   </si>
@@ -169,9 +169,6 @@
     <t>6, 2, 3, 2</t>
   </si>
   <si>
-    <t>Empty group in modal clustering</t>
-  </si>
-  <si>
     <t>3, 4, 3, 3</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>Olive2</t>
   </si>
   <si>
-    <t>6, 2, 2, 2, 2, 2</t>
-  </si>
-  <si>
     <t>5, 5, 5, 5, 5, 5</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t>50 extra variables of Gaussian Noise</t>
   </si>
   <si>
-    <t>100 extra variables of Gaussian Noise</t>
-  </si>
-  <si>
     <t>Pareto Scaling</t>
   </si>
   <si>
@@ -286,9 +277,6 @@
     <t>2, 2, 2</t>
   </si>
   <si>
-    <t>Pareto Scaling, Rho=0.75, alpha.d1=5, alpha.d2=10</t>
-  </si>
-  <si>
     <t>Error Area (%)</t>
   </si>
   <si>
@@ -322,9 +310,6 @@
     <t>Adj. Rand Cinzia</t>
   </si>
   <si>
-    <t>Rho=0.7</t>
-  </si>
-  <si>
     <t>Support for G=4, alpha.d1=3, alpha.d2=6</t>
   </si>
   <si>
@@ -389,6 +374,45 @@
   </si>
   <si>
     <t>alpha.d1=4, alpha.d2=8</t>
+  </si>
+  <si>
+    <t>2, 2, 2, 2, 2, 2</t>
+  </si>
+  <si>
+    <t>Adj. Rand</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 1</t>
+  </si>
+  <si>
+    <t>2, 1, 1, 1, 2</t>
+  </si>
+  <si>
+    <t>10 extra observations of Gaussian Noise</t>
+  </si>
+  <si>
+    <t>100 extra observations of Gaussian Noise</t>
+  </si>
+  <si>
+    <t>50 extra observations of Gaussian Noise</t>
+  </si>
+  <si>
+    <t>100 extra variables of Gaussian Noise  - one big group beyond this point</t>
+  </si>
+  <si>
+    <t>4 + 2 x 10</t>
+  </si>
+  <si>
+    <t>3 + 2 x 8</t>
+  </si>
+  <si>
+    <t>2 x 7</t>
+  </si>
+  <si>
+    <t>6, 2, 2, 2, 2</t>
+  </si>
+  <si>
+    <t>Pareto Scaling, alpha.d1=5, alpha.d2=10</t>
   </si>
 </sst>
 </file>
@@ -456,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -631,11 +655,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -754,9 +787,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,6 +811,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1157,13 +1209,14 @@
     <col min="7" max="7" width="6.68359375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.68359375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.68359375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1192,58 +1245,64 @@
         <v>3</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="50"/>
-    </row>
-    <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="43">
+      <c r="M1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="42">
         <v>50000</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="42">
         <v>9824.93</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>8.9600000000000009</v>
       </c>
-      <c r="F2" s="43">
-        <v>0</v>
-      </c>
-      <c r="G2" s="48">
+      <c r="F2" s="42">
+        <v>0</v>
+      </c>
+      <c r="G2" s="47">
         <v>2</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="42">
         <v>4</v>
       </c>
-      <c r="I2" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="43">
+      <c r="I2" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="42">
+        <v>9.5699999999999993E-2</v>
+      </c>
+      <c r="K2" s="42">
         <v>27.78</v>
       </c>
-      <c r="K2" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
@@ -1269,22 +1328,25 @@
         <v>3</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J3" s="14">
+        <v>0.89439999999999997</v>
+      </c>
+      <c r="K3" s="14">
         <v>5.56</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="M3" s="20">
+      <c r="L3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" s="20">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -1313,20 +1375,23 @@
         <v>7</v>
       </c>
       <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
         <v>76.19</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="20">
+      <c r="N4" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1345,17 +1410,18 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="19" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="20">
+      <c r="N5" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1374,16 +1440,17 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="19" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="20">
+      <c r="N6" s="20">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="17" t="s">
         <v>18</v>
       </c>
@@ -1404,16 +1471,17 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="21" t="s">
+      <c r="K7" s="6"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="22" t="b">
+      <c r="N7" s="22" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="40" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1433,9 +1501,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" s="6"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="37" t="s">
         <v>20</v>
       </c>
@@ -1456,11 +1525,12 @@
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1472,9 +1542,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1487,13 +1559,13 @@
     <col min="7" max="7" width="5.68359375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.89453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.68359375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.15625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.26171875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.26171875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.41796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.7890625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.05078125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.9453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.62890625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1512,10 +1584,10 @@
         <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>30</v>
@@ -1533,74 +1605,74 @@
         <v>3</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="P1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="50"/>
+      <c r="Q1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="1:18" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="43">
+      <c r="A2" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="42">
         <v>50000</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="42">
         <v>1991.42</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="42">
         <v>1</v>
       </c>
-      <c r="F2" s="44">
-        <f t="shared" ref="F2:F14" si="0">D2/$D$3</f>
+      <c r="F2" s="43">
+        <f t="shared" ref="F2:F11" si="0">D2/$D$3</f>
         <v>1.097449010520283</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2" s="44">
         <v>4.5599999999999996</v>
       </c>
-      <c r="H2" s="43">
-        <v>0</v>
-      </c>
-      <c r="I2" s="46" t="s">
+      <c r="H2" s="42">
+        <v>0</v>
+      </c>
+      <c r="I2" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="43">
-        <v>5</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="43">
+      <c r="J2" s="42">
+        <v>5</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="42">
         <v>0.93579999999999997</v>
       </c>
-      <c r="M2" s="43">
+      <c r="M2" s="42">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N2" s="43">
+      <c r="N2" s="42">
         <v>8.57</v>
       </c>
-      <c r="O2" s="43">
+      <c r="O2" s="42">
         <v>0.7</v>
       </c>
-      <c r="P2" s="47" t="s">
-        <v>98</v>
+      <c r="P2" s="46" t="s">
+        <v>93</v>
       </c>
       <c r="Q2" s="19" t="s">
         <v>25</v>
@@ -1656,14 +1728,12 @@
       <c r="O3" s="14">
         <v>0.7</v>
       </c>
-      <c r="P3" s="13" t="s">
-        <v>97</v>
-      </c>
+      <c r="P3" s="13"/>
       <c r="Q3" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R3" s="20">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1699,7 +1769,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" s="4">
         <v>0.51639999999999997</v>
@@ -1714,7 +1784,7 @@
         <v>28.85</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="19" t="s">
         <v>34</v>
@@ -1753,10 +1823,10 @@
         <v>13</v>
       </c>
       <c r="J5" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="L5" s="4">
         <v>0.90369999999999995</v>
@@ -1770,9 +1840,7 @@
       <c r="O5" s="4">
         <v>7.52</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="19" t="s">
         <v>35</v>
       </c>
@@ -1813,7 +1881,7 @@
         <v>6</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L6" s="6">
         <v>0.51529999999999998</v>
@@ -1828,7 +1896,7 @@
         <v>29.02</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>36</v>
@@ -1885,7 +1953,7 @@
         <v>43.53</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Q7" s="21" t="s">
         <v>37</v>
@@ -1927,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L8" s="6">
         <v>0.81920000000000004</v>
@@ -1942,7 +2010,7 @@
         <v>26.05</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2042,56 +2110,57 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="52">
         <v>305.63499999999999</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="52">
         <v>63</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="53">
         <f t="shared" si="0"/>
         <v>0.16843198739109111</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="G11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="5">
-        <v>5</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="J11" s="52">
+        <v>5</v>
+      </c>
+      <c r="K11" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="L11" s="51">
         <v>0.58860000000000001</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="51">
         <v>0.59130000000000005</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="51">
         <v>33.56</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="51">
         <v>29.02</v>
       </c>
+      <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2100,12 +2169,18 @@
       <c r="C12" s="5">
         <v>50000</v>
       </c>
+      <c r="D12" s="5">
+        <v>2475.5500000000002</v>
+      </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F12:F17" si="1">D12/$D$3</f>
+        <v>1.3642475710766622</v>
+      </c>
+      <c r="G12" s="50">
+        <v>4.55</v>
       </c>
       <c r="H12" s="5">
         <v>0</v>
@@ -2113,12 +2188,30 @@
       <c r="I12" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="J12" s="5">
+        <v>6</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" s="50">
+        <v>0.87560000000000004</v>
+      </c>
+      <c r="M12" s="50">
+        <v>0.93659999999999999</v>
+      </c>
+      <c r="N12" s="50">
+        <v>22.03</v>
+      </c>
+      <c r="O12" s="50">
+        <v>13.64</v>
+      </c>
       <c r="P12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2127,12 +2220,18 @@
       <c r="C13" s="5">
         <v>50000</v>
       </c>
+      <c r="D13" s="48">
+        <v>5664.07</v>
+      </c>
       <c r="E13" s="5">
         <v>1</v>
       </c>
       <c r="F13" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.1214048352520405</v>
+      </c>
+      <c r="G13" s="48">
+        <v>4.55</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
@@ -2140,12 +2239,30 @@
       <c r="I13" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="J13" s="48">
+        <v>5</v>
+      </c>
+      <c r="K13" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="48">
+        <v>0.68430000000000002</v>
+      </c>
+      <c r="M13" s="48">
+        <v>0.73650000000000004</v>
+      </c>
+      <c r="N13" s="48">
+        <v>22.55</v>
+      </c>
+      <c r="O13" s="48">
+        <v>14.69</v>
+      </c>
       <c r="P13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2154,12 +2271,18 @@
       <c r="C14" s="5">
         <v>50000</v>
       </c>
+      <c r="D14" s="48">
+        <v>9377.56</v>
+      </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.1678671214985199</v>
+      </c>
+      <c r="G14" s="48">
+        <v>4.5599999999999996</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
@@ -2167,13 +2290,184 @@
       <c r="I14" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="J14" s="48">
+        <v>4</v>
+      </c>
+      <c r="K14" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="48">
+        <v>0.68030000000000002</v>
+      </c>
+      <c r="M14" s="48">
+        <v>0.73340000000000005</v>
+      </c>
+      <c r="N14" s="48">
+        <v>17.13</v>
+      </c>
+      <c r="O14" s="48">
+        <v>17.66</v>
+      </c>
       <c r="P14" t="s">
-        <v>78</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5">
+        <v>50000</v>
+      </c>
+      <c r="D15" s="48">
+        <v>2212.71</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="39">
+        <f t="shared" si="1"/>
+        <v>1.2193994235612453</v>
+      </c>
+      <c r="G15" s="48">
+        <v>4.53</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="48">
+        <v>11</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="48">
+        <v>0.80010000000000003</v>
+      </c>
+      <c r="M15" s="48">
+        <v>0.85819999999999996</v>
+      </c>
+      <c r="N15" s="48">
+        <v>22.85</v>
+      </c>
+      <c r="O15" s="48">
+        <v>14.6</v>
+      </c>
+      <c r="P15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1" t="s">
-        <v>92</v>
+      <c r="A16" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>50000</v>
+      </c>
+      <c r="D16" s="48">
+        <v>2222.5700000000002</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="39">
+        <f t="shared" si="1"/>
+        <v>1.2248331579034384</v>
+      </c>
+      <c r="G16" s="48">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="48">
+        <v>9</v>
+      </c>
+      <c r="K16" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="L16" s="48">
+        <v>0.51829999999999998</v>
+      </c>
+      <c r="M16" s="48">
+        <v>0.56320000000000003</v>
+      </c>
+      <c r="N16" s="48">
+        <v>37.78</v>
+      </c>
+      <c r="O16" s="48">
+        <v>30.23</v>
+      </c>
+      <c r="P16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="48">
+        <v>4189.93</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="39">
+        <f t="shared" si="1"/>
+        <v>2.3090229748868891</v>
+      </c>
+      <c r="G17" s="48">
+        <v>4.41</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="48">
+        <v>7</v>
+      </c>
+      <c r="K17" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" s="48">
+        <v>0.62419999999999998</v>
+      </c>
+      <c r="M17" s="48">
+        <v>0.62319999999999998</v>
+      </c>
+      <c r="N17" s="48">
+        <v>30.36</v>
+      </c>
+      <c r="O17" s="48">
+        <v>28.12</v>
+      </c>
+      <c r="P17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2190,10 +2484,10 @@
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2221,19 +2515,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>21</v>
@@ -2395,7 +2689,7 @@
         <v>28.85</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2555,7 +2849,7 @@
         <v>29.19</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2584,7 +2878,7 @@
         <v>29.02</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2640,7 +2934,7 @@
         <v>43.53</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2651,10 +2945,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E17" s="5">
         <v>0.81920000000000004</v>
@@ -2677,10 +2971,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E18" s="5">
         <v>0.82020000000000004</v>
@@ -2703,10 +2997,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E19" s="5">
         <v>0.9304</v>
@@ -2721,7 +3015,7 @@
         <v>6.99</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2732,10 +3026,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E20" s="5">
         <v>0.90449999999999997</v>
@@ -2750,7 +3044,7 @@
         <v>6.99</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2761,10 +3055,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E21" s="5">
         <v>0.9284</v>
@@ -2787,10 +3081,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E22" s="5">
         <v>0.68010000000000004</v>
@@ -2813,10 +3107,10 @@
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E23" s="5">
         <v>0.5474</v>
@@ -2839,10 +3133,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E24" s="3">
         <v>0.80300000000000005</v>
@@ -3196,7 +3490,7 @@
         <v>26.05</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4447,7 +4741,7 @@
         <v>9.27</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4578,10 +4872,10 @@
       <c r="K1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="50"/>
+      <c r="L1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -4609,7 +4903,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="6">
         <v>79.150000000000006</v>
@@ -4655,7 +4949,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M3" s="20">
         <v>0.75</v>
@@ -4687,13 +4981,13 @@
         <v>5</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" s="6">
         <v>3.33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>34</v>
@@ -4703,38 +4997,38 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="43">
+      <c r="A5" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="42">
         <v>50000</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <v>1991.42</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="44">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F5" s="43">
-        <v>0</v>
-      </c>
-      <c r="G5" s="46" t="s">
+      <c r="F5" s="42">
+        <v>0</v>
+      </c>
+      <c r="G5" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="43">
-        <v>5</v>
-      </c>
-      <c r="I5" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="43">
+      <c r="H5" s="42">
+        <v>5</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="42">
         <v>0.7</v>
       </c>
-      <c r="K5" s="47" t="s">
-        <v>89</v>
+      <c r="K5" s="46" t="s">
+        <v>85</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>35</v>
@@ -4775,7 +5069,7 @@
         <v>0.7</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>36</v>
@@ -4932,7 +5226,7 @@
   <dimension ref="B1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4954,47 +5248,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="57"/>
+    </row>
+    <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="50"/>
-    </row>
-    <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="60" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="57" t="s">
+      <c r="F2" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="G2" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="H2" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="I2" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="J2" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="K2" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="L2" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="M2" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="65" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="19" t="s">
@@ -5005,31 +5299,31 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
       <c r="P3" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="20">
         <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="52"/>
+      <c r="B4" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="59"/>
       <c r="D4" s="24">
         <v>0.5</v>
       </c>
@@ -5037,25 +5331,25 @@
         <v>3</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="27">
         <v>4</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" s="27">
         <v>4</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="27">
         <v>4</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M4" s="28">
         <v>327.02999999999997</v>
@@ -5071,8 +5365,8 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="53"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="24">
         <v>1</v>
       </c>
@@ -5080,25 +5374,25 @@
         <v>3</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="28">
         <v>4</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="28">
         <v>4</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" s="28">
         <v>4</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" s="28">
         <v>328.11</v>
@@ -5114,8 +5408,8 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="24">
         <v>5</v>
       </c>
@@ -5123,25 +5417,25 @@
         <v>3</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="28">
         <v>4</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="28">
         <v>4</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="28">
         <v>4</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M6" s="28">
         <v>330.5</v>
@@ -5157,34 +5451,34 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="33">
         <v>3</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="34">
         <v>4</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="34">
         <v>3</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" s="34">
         <v>4</v>
       </c>
       <c r="L7" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M7" s="34">
         <v>327.56</v>
@@ -5200,10 +5494,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="52"/>
+      <c r="B8" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="59"/>
       <c r="D8" s="24">
         <v>0.5</v>
       </c>
@@ -5211,25 +5505,25 @@
         <v>3</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="36">
         <v>5</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="36">
+        <v>5</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="36">
+        <v>5</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="I8" s="36">
-        <v>5</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="36">
-        <v>5</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="M8" s="25">
         <v>361.66</v>
@@ -5239,8 +5533,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="24">
         <v>1</v>
       </c>
@@ -5248,25 +5542,25 @@
         <v>3</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="36">
         <v>5</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="36">
         <v>5</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" s="36">
         <v>5</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M9" s="30">
         <v>363.06</v>
@@ -5276,8 +5570,8 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="24">
         <v>5</v>
       </c>
@@ -5285,25 +5579,25 @@
         <v>3</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="36">
         <v>5</v>
       </c>
       <c r="H10" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="36">
+        <v>5</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="36">
+        <v>5</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="I10" s="36">
-        <v>5</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="36">
-        <v>5</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="M10" s="30">
         <v>367.44</v>
@@ -5313,34 +5607,34 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="36">
         <v>3</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" s="36">
         <v>5</v>
       </c>
       <c r="H11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="36">
+        <v>5</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="36">
+        <v>5</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="I11" s="36">
-        <v>5</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="36">
-        <v>5</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="M11" s="33">
         <v>366.57</v>
@@ -5350,10 +5644,10 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="52"/>
+      <c r="B12" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="59"/>
       <c r="D12" s="26">
         <v>0.5</v>
       </c>
@@ -5361,25 +5655,25 @@
         <v>3</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="27">
         <v>5</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="27">
         <v>5</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" s="27">
         <v>5</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M12" s="28">
         <v>555.82000000000005</v>
@@ -5389,8 +5683,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="24">
         <v>1</v>
       </c>
@@ -5398,25 +5692,25 @@
         <v>3</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="28">
         <v>5</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="28">
         <v>5</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="28">
         <v>5</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M13" s="28">
         <v>558.52</v>
@@ -5426,8 +5720,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="24">
         <v>5</v>
       </c>
@@ -5435,25 +5729,25 @@
         <v>3</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" s="28">
         <v>5</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="28">
         <v>5</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" s="28">
         <v>5</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M14" s="28">
         <v>560.75</v>
@@ -5463,34 +5757,34 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="33">
         <v>3</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="34">
         <v>5</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I15" s="34">
         <v>5</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="34">
         <v>5</v>
       </c>
       <c r="L15" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M15" s="34">
         <v>560.46</v>
@@ -5679,7 +5973,7 @@
         <v>33.56</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Added RatBrain data, added plots with/without colMeans to Brain/Urine, edited calculation of colMeans to use by(). Edited Notes.pdf to reflect Claire's comments, incl. Ghost (2008) parameter expanded FA reference, improved use of \citet/\citep/Section etc., and diagram of typical MGP prior.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="131">
   <si>
     <t>Data</t>
   </si>
@@ -413,6 +413,15 @@
   </si>
   <si>
     <t>Pareto Scaling, alpha.d1=5, alpha.d2=10</t>
+  </si>
+  <si>
+    <t>Brain</t>
+  </si>
+  <si>
+    <t>3, 3, 3, 15</t>
+  </si>
+  <si>
+    <t>2, 2, 2, 2</t>
   </si>
 </sst>
 </file>
@@ -422,7 +431,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,13 +463,6 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -787,12 +789,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -876,6 +872,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1192,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1253,46 +1255,46 @@
       <c r="L1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="57"/>
+      <c r="N1" s="55"/>
     </row>
     <row r="2" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="42">
+      <c r="B2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="40">
         <v>50000</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="40">
         <v>9824.93</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="42">
         <v>8.9600000000000009</v>
       </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="47">
+      <c r="F2" s="40">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45">
         <v>2</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="40">
         <v>4</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="40">
         <v>9.5699999999999993E-2</v>
       </c>
-      <c r="K2" s="42">
+      <c r="K2" s="40">
         <v>27.78</v>
       </c>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="44" t="s">
         <v>76</v>
       </c>
       <c r="M2" s="19" t="s">
@@ -1347,41 +1349,41 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="D4" s="8">
-        <v>203019.97</v>
-      </c>
-      <c r="E4" s="8">
-        <v>5.62</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>5</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8">
-        <v>7</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>76.19</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>114</v>
+      <c r="A4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="14">
+        <v>50000</v>
+      </c>
+      <c r="D4" s="14">
+        <v>7059.95</v>
+      </c>
+      <c r="E4" s="15">
+        <v>15.98</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="18">
+        <v>4</v>
+      </c>
+      <c r="H4" s="14">
+        <v>4</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="K4" s="14">
+        <v>24.24</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="M4" s="19" t="s">
         <v>34</v>
@@ -1391,28 +1393,42 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6">
-        <v>10000</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="1"/>
+      <c r="A5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="14">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3618.23</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18">
+        <v>4</v>
+      </c>
+      <c r="H5" s="14">
+        <v>4</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="K5" s="14">
+        <v>24.24</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="M5" s="19" t="s">
         <v>35</v>
       </c>
@@ -1421,28 +1437,42 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
         <v>10000</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="2"/>
+      <c r="D6" s="8">
+        <v>203019.97</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5.62</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>7</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>76.19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="M6" s="19" t="s">
         <v>36</v>
       </c>
@@ -1451,8 +1481,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="17" t="s">
-        <v>18</v>
+      <c r="A7" s="69" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -1462,17 +1492,17 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="6"/>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="21" t="s">
         <v>37</v>
       </c>
@@ -1481,10 +1511,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6">
@@ -1492,41 +1522,89 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>4</v>
-      </c>
-      <c r="H8" s="6"/>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="38">
+      <c r="B11" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="34">
         <v>10000</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38">
-        <v>0</v>
-      </c>
-      <c r="G9" s="38">
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34">
         <v>4</v>
       </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="1"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1619,59 +1697,59 @@
       <c r="P1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="57"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:18" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="42">
+      <c r="B2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="40">
         <v>50000</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="40">
         <v>1991.42</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="40">
         <v>1</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="41">
         <f t="shared" ref="F2:F11" si="0">D2/$D$3</f>
         <v>1.097449010520283</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="42">
         <v>4.5599999999999996</v>
       </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="45" t="s">
+      <c r="H2" s="40">
+        <v>0</v>
+      </c>
+      <c r="I2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="42">
-        <v>5</v>
-      </c>
-      <c r="K2" s="42" t="s">
+      <c r="J2" s="40">
+        <v>5</v>
+      </c>
+      <c r="K2" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="42">
+      <c r="L2" s="40">
         <v>0.93579999999999997</v>
       </c>
-      <c r="M2" s="42">
+      <c r="M2" s="40">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N2" s="42">
+      <c r="N2" s="40">
         <v>8.57</v>
       </c>
-      <c r="O2" s="42">
+      <c r="O2" s="40">
         <v>0.7</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="P2" s="44" t="s">
         <v>93</v>
       </c>
       <c r="Q2" s="19" t="s">
@@ -2111,56 +2189,56 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="52">
+      <c r="C11" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="50">
         <v>305.63499999999999</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="50">
         <v>63</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="51">
         <f t="shared" si="0"/>
         <v>0.16843198739109111</v>
       </c>
-      <c r="G11" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="54" t="s">
+      <c r="G11" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="52">
-        <v>5</v>
-      </c>
-      <c r="K11" s="52" t="s">
+      <c r="J11" s="50">
+        <v>5</v>
+      </c>
+      <c r="K11" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="51">
+      <c r="L11" s="49">
         <v>0.58860000000000001</v>
       </c>
-      <c r="M11" s="51">
+      <c r="M11" s="49">
         <v>0.59130000000000005</v>
       </c>
-      <c r="N11" s="51">
+      <c r="N11" s="49">
         <v>33.56</v>
       </c>
-      <c r="O11" s="51">
+      <c r="O11" s="49">
         <v>29.02</v>
       </c>
-      <c r="P11" s="55"/>
+      <c r="P11" s="53"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2179,7 +2257,7 @@
         <f t="shared" ref="F12:F17" si="1">D12/$D$3</f>
         <v>1.3642475710766622</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G12" s="48">
         <v>4.55</v>
       </c>
       <c r="H12" s="5">
@@ -2191,19 +2269,19 @@
       <c r="J12" s="5">
         <v>6</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="L12" s="50">
+      <c r="L12" s="48">
         <v>0.87560000000000004</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="48">
         <v>0.93659999999999999</v>
       </c>
-      <c r="N12" s="50">
+      <c r="N12" s="48">
         <v>22.03</v>
       </c>
-      <c r="O12" s="50">
+      <c r="O12" s="48">
         <v>13.64</v>
       </c>
       <c r="P12" t="s">
@@ -2211,7 +2289,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2220,7 +2298,7 @@
       <c r="C13" s="5">
         <v>50000</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="46">
         <v>5664.07</v>
       </c>
       <c r="E13" s="5">
@@ -2230,7 +2308,7 @@
         <f t="shared" si="1"/>
         <v>3.1214048352520405</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="46">
         <v>4.55</v>
       </c>
       <c r="H13" s="5">
@@ -2239,22 +2317,22 @@
       <c r="I13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="48">
-        <v>5</v>
-      </c>
-      <c r="K13" s="48" t="s">
+      <c r="J13" s="46">
+        <v>5</v>
+      </c>
+      <c r="K13" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="46">
         <v>0.68430000000000002</v>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="46">
         <v>0.73650000000000004</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="46">
         <v>22.55</v>
       </c>
-      <c r="O13" s="48">
+      <c r="O13" s="46">
         <v>14.69</v>
       </c>
       <c r="P13" t="s">
@@ -2262,7 +2340,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2271,7 +2349,7 @@
       <c r="C14" s="5">
         <v>50000</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="46">
         <v>9377.56</v>
       </c>
       <c r="E14" s="5">
@@ -2281,7 +2359,7 @@
         <f t="shared" si="1"/>
         <v>5.1678671214985199</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="46">
         <v>4.5599999999999996</v>
       </c>
       <c r="H14" s="5">
@@ -2290,22 +2368,22 @@
       <c r="I14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="48">
+      <c r="J14" s="46">
         <v>4</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="46">
         <v>0.68030000000000002</v>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="46">
         <v>0.73340000000000005</v>
       </c>
-      <c r="N14" s="48">
+      <c r="N14" s="46">
         <v>17.13</v>
       </c>
-      <c r="O14" s="48">
+      <c r="O14" s="46">
         <v>17.66</v>
       </c>
       <c r="P14" t="s">
@@ -2313,7 +2391,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2322,7 +2400,7 @@
       <c r="C15" s="5">
         <v>50000</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="46">
         <v>2212.71</v>
       </c>
       <c r="E15" s="5">
@@ -2332,7 +2410,7 @@
         <f t="shared" si="1"/>
         <v>1.2193994235612453</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="46">
         <v>4.53</v>
       </c>
       <c r="H15" s="5">
@@ -2341,22 +2419,22 @@
       <c r="I15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="48">
+      <c r="J15" s="46">
         <v>11</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="48">
+      <c r="L15" s="46">
         <v>0.80010000000000003</v>
       </c>
-      <c r="M15" s="48">
+      <c r="M15" s="46">
         <v>0.85819999999999996</v>
       </c>
-      <c r="N15" s="48">
+      <c r="N15" s="46">
         <v>22.85</v>
       </c>
-      <c r="O15" s="48">
+      <c r="O15" s="46">
         <v>14.6</v>
       </c>
       <c r="P15" t="s">
@@ -2364,7 +2442,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2373,7 +2451,7 @@
       <c r="C16" s="5">
         <v>50000</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="46">
         <v>2222.5700000000002</v>
       </c>
       <c r="E16" s="5">
@@ -2383,7 +2461,7 @@
         <f t="shared" si="1"/>
         <v>1.2248331579034384</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="46">
         <v>4.4800000000000004</v>
       </c>
       <c r="H16" s="5">
@@ -2392,22 +2470,22 @@
       <c r="I16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="48">
+      <c r="J16" s="46">
         <v>9</v>
       </c>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="46">
         <v>0.51829999999999998</v>
       </c>
-      <c r="M16" s="48">
+      <c r="M16" s="46">
         <v>0.56320000000000003</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="46">
         <v>37.78</v>
       </c>
-      <c r="O16" s="48">
+      <c r="O16" s="46">
         <v>30.23</v>
       </c>
       <c r="P16" t="s">
@@ -2415,7 +2493,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2424,7 +2502,7 @@
       <c r="C17" s="5">
         <v>50000</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="46">
         <v>4189.93</v>
       </c>
       <c r="E17" s="5">
@@ -2434,7 +2512,7 @@
         <f t="shared" si="1"/>
         <v>2.3090229748868891</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="46">
         <v>4.41</v>
       </c>
       <c r="H17" s="5">
@@ -2443,22 +2521,22 @@
       <c r="I17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="48">
+      <c r="J17" s="46">
         <v>7</v>
       </c>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="48">
+      <c r="L17" s="46">
         <v>0.62419999999999998</v>
       </c>
-      <c r="M17" s="48">
+      <c r="M17" s="46">
         <v>0.62319999999999998</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="46">
         <v>30.36</v>
       </c>
-      <c r="O17" s="48">
+      <c r="O17" s="46">
         <v>28.12</v>
       </c>
       <c r="P17" t="s">
@@ -4872,10 +4950,10 @@
       <c r="K1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="57"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
@@ -4997,37 +5075,37 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="42">
+      <c r="B5" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="40">
         <v>50000</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="40">
         <v>1991.42</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="42">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F5" s="42">
-        <v>0</v>
-      </c>
-      <c r="G5" s="45" t="s">
+      <c r="F5" s="40">
+        <v>0</v>
+      </c>
+      <c r="G5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="42">
-        <v>5</v>
-      </c>
-      <c r="I5" s="42" t="s">
+      <c r="H5" s="40">
+        <v>5</v>
+      </c>
+      <c r="I5" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="40">
         <v>0.7</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="44" t="s">
         <v>85</v>
       </c>
       <c r="L5" s="19" t="s">
@@ -5248,47 +5326,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="P1" s="56" t="s">
+      <c r="P1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="57"/>
+      <c r="Q1" s="55"/>
     </row>
     <row r="2" spans="2:17" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="J2" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="K2" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="64" t="s">
+      <c r="L2" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="65" t="s">
+      <c r="M2" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="65" t="s">
+      <c r="N2" s="63" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="19" t="s">
@@ -5299,19 +5377,19 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
       <c r="P3" s="19" t="s">
         <v>78</v>
       </c>
@@ -5320,10 +5398,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="24">
         <v>0.5</v>
       </c>
@@ -5365,8 +5443,8 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="60"/>
-      <c r="C5" s="61"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="24">
         <v>1</v>
       </c>
@@ -5408,8 +5486,8 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="60"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="24">
         <v>5</v>
       </c>
@@ -5451,8 +5529,8 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="62"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="32" t="s">
         <v>64</v>
       </c>
@@ -5494,10 +5572,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="24">
         <v>0.5</v>
       </c>
@@ -5533,8 +5611,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="24">
         <v>1</v>
       </c>
@@ -5570,8 +5648,8 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="60"/>
-      <c r="C10" s="61"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="24">
         <v>5</v>
       </c>
@@ -5607,8 +5685,8 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="32" t="s">
         <v>64</v>
       </c>
@@ -5644,10 +5722,10 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="59"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="26">
         <v>0.5</v>
       </c>
@@ -5683,8 +5761,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="24">
         <v>1</v>
       </c>
@@ -5720,8 +5798,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="60"/>
-      <c r="C14" s="61"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="24">
         <v>5</v>
       </c>
@@ -5757,8 +5835,8 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="62"/>
-      <c r="C15" s="63"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="32" t="s">
         <v>64</v>
       </c>

</xml_diff>